<commit_message>
add cal equip property's interface
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/Item.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/Item.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050"/>
+    <workbookView windowWidth="27765" windowHeight="15450"/>
   </bookViews>
   <sheets>
     <sheet name="Property" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54">
   <si>
     <t>Id</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>名字</t>
+  </si>
+  <si>
+    <t>HeroType</t>
+  </si>
+  <si>
+    <t>归属英雄类型，力敏智</t>
   </si>
 </sst>
 </file>
@@ -180,10 +186,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -195,6 +201,73 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -209,31 +282,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -254,32 +313,32 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -290,59 +349,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -359,187 +365,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -550,6 +556,35 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -583,6 +618,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -594,35 +638,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -641,162 +656,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -877,7 +883,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font/>
       <fill>
         <patternFill patternType="none"/>
       </fill>
@@ -1222,10 +1227,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F20"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1881,10 +1886,42 @@
         <v>51</v>
       </c>
     </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F20 F21:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F21 F2:F20 F22:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>